<commit_message>
changing_grid and bootstraps data
</commit_message>
<xml_diff>
--- a/data/6_tables/tables_appendix/App_Table3_CI_with_cis_new.xlsx
+++ b/data/6_tables/tables_appendix/App_Table3_CI_with_cis_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcchen\Documents\GitHub\mvpf-climate\data\6_tables\tables_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA08C0-1D9A-4AD5-B447-6CF39569AF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD0B702-EB9E-4A31-9474-7BDC711C1ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896"/>
   </bookViews>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BF7382-BA68-4FFF-972D-6F46E493258F}">
   <dimension ref="F1:AN138"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="C108" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AC125" sqref="AC125"/>
+    <sheetView tabSelected="true" topLeftCell="C95" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultColWidth="9.109375" defaultRowHeight="28.8" x14ac:dyDescent="0.3"/>
@@ -4938,8 +4938,14 @@
         <f>data_export!B81</f>
         <v>0.84163074640426783</v>
       </c>
-      <c r="O108" s="31"/>
-      <c r="T108" s="31"/>
+      <c r="O108" s="31">
+        <f>data_export!E81</f>
+        <v>0.87774564090825169</v>
+      </c>
+      <c r="T108" s="31">
+        <f>data_export!H81</f>
+        <v>0.79655280626066549</v>
+      </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="109" ht="10.2" customHeight="true" x14ac:dyDescent="0.3">
       <c r="H109" s="28"/>
@@ -6012,8 +6018,8 @@
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E91" sqref="E91"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8652,25 +8658,25 @@
         <v>323.45293945283288</v>
       </c>
       <c r="C93" s="1">
-        <v>12.638619422912598</v>
+        <v>311.78076171875</v>
       </c>
       <c r="D93" s="1">
-        <v>112.08157348632813</v>
+        <v>336.26370239257813</v>
       </c>
       <c r="E93" s="1">
         <v>36.928823958820452</v>
       </c>
       <c r="F93" s="1">
-        <v>7.2278647422790527</v>
+        <v>34.188835144042969</v>
       </c>
       <c r="G93" s="1">
-        <v>23.538509368896484</v>
+        <v>39.936092376708984</v>
       </c>
       <c r="H93" s="1">
         <v>99999</v>
       </c>
       <c r="I93" s="1">
-        <v>20.432701110839844</v>
+        <v>99999</v>
       </c>
       <c r="J93" s="1">
         <v>99999</v>

</xml_diff>